<commit_message>
Leker med data i R.Rmd
</commit_message>
<xml_diff>
--- a/DATA/langtidstest_pilot_data.xlsx
+++ b/DATA/langtidstest_pilot_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows User\Documents\Master\Test-data-TR032REPEAT\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8E77077-58BB-4235-A52E-E3B8CDB468EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA98B00E-C066-4312-A2FB-3C579FA94AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{52B45812-C777-4D4D-B51E-08354AA17B25}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <dimension ref="A1:BL19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BE13" sqref="BE13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>